<commit_message>
Completed implementing the Excel type provider using the ExcelDataReader library
</commit_message>
<xml_diff>
--- a/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
+++ b/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>String</t>
-  </si>
-  <si>
-    <t>Int</t>
   </si>
   <si>
     <t>Float</t>
@@ -69,10 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -376,18 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,28 +394,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="b">
+      <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D2" s="3">
         <f ca="1">NOW()</f>
-        <v>41448.509828703704</v>
+        <v>41448.658352430553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing the date column for now. The Excel type provider reports an error. - relates to issue #236
</commit_message>
<xml_diff>
--- a/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
+++ b/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="8595" windowHeight="8760"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>String</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -73,7 +70,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -86,9 +83,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,7 +123,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -198,7 +195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -375,10 +372,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D2" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -393,9 +390,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -407,10 +401,7 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
-        <f ca="1">NOW()</f>
-        <v>41448.658352430553</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -424,7 +415,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -436,7 +427,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Addressing unit test failures for the Excel type provider
</commit_message>
<xml_diff>
--- a/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
+++ b/tests/FSharpx.TypeProviders.Excel.Tests/DataTypes.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\Documents\GitHub\fsharpx\tests\FSharpx.TypeProviders.Excel.Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="8595" windowHeight="8760"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>String</t>
   </si>
@@ -28,12 +33,26 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,14 +82,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -78,14 +99,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -123,9 +147,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -160,7 +184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -369,18 +393,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,8 +415,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -401,7 +435,17 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <f ca="1">NOW()</f>
+        <v>41449.359279166667</v>
+      </c>
+      <c r="E2" s="4">
+        <f ca="1" xml:space="preserve"> NOW()</f>
+        <v>41449.359279166667</v>
+      </c>
+      <c r="F2" s="5">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -415,7 +459,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -427,7 +471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>